<commit_message>
related work about software defined awareness.
</commit_message>
<xml_diff>
--- a/软件定义感知/content.xlsx
+++ b/软件定义感知/content.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\实验室相关\人机物\论文\RelatedWorks\软件定义建模与执行\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lixiangmin/RelatedWorks/软件定义感知/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37825D21-3B63-444D-BF7A-6592D2DE7FC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21231F7D-E54A-9B4B-B3B3-D550F03CAEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="223" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="223" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Reactive Microservices for the Internet of Things: A case study in Fog Computing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,9 +39,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://dl.acm.org/doi/10.1145/3297280.3297402</t>
-  </si>
-  <si>
     <t>Ind</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -53,15 +47,175 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The Future Internet will be able to connect most of the objects that are not yet connected on the current Internet. The Internet of Things (IoT) is an important part of the Future Internet and involves connectivity between several physical and virtual objects, allowing the emergence of new services and applications. These intelligent objects, along with their tasks, constitute domain-specific applications (vertical markets), while ubiquitous and analytic services form independent domain services (horizontal markets). The development of these applications and services in these markets brings challenges such as deployment, scalability, integration, interoperability, mobility and performance. Recent research indicates that Microservices has been successfully applied by companies such as Netflix and SoundCloud to address some of these issues in their cloud computing applications. However, in the field of IoT, the use of Microservices to deal with these challenges still presents unresolved issues. In this paper, we present a reactive Microservices architecture and apply it in a Fog Computing case study to investigate these challenges at the edge of the network. Finally, we evaluate our proposal from the perspective of performance of Microservices provided by intelligent objects (IoT gateways) at the edge of the network.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C. de Santana</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>First Author</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">A framework of smart homes connected devices using Internet of Things </t>
+  </si>
+  <si>
+    <t>Internet of Things (IoT) is an extensive network of connected components working in unison by coordinating, acknowledging and sharing the resources in the network. Smart frameworks provide an optimal ambient environment for the occupants in smart homes, offices and surrounding environment. The proposed smart home framework incorporates multiple heterogeneous devices that communicate with each other and establish a collaborative network. In this framework, the server accepts incoming requests from connected devices and support interoperability across the connected devices. Simulation for IoT Smart Home includes components such as the centralized server, home security, smart phones, smart thermostat, centralized air condition, connected lights, windows and ventilation control, smart TV and smart fridge. Smart home simulations based device initialization (between server and device), data exchange sequence, module log and event log are given in the proposed framework.</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/7918794</t>
+  </si>
+  <si>
+    <t>M. Bala Krishna</t>
+  </si>
+  <si>
+    <t>Sang Gi Hong</t>
+  </si>
+  <si>
+    <t>This paper proposes a software framework and hardware architecture to exchange the binaries and profiles from smartphones to IoT devices and reprogram devices with smartphones. This scheme, when included in a system of smartphones interconnected with locally deployed IoT devices in wired or wireless manners, can be used to implement a practical updater.</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/7177805</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A smartphone connected software updating framework for IoT devices</t>
+  </si>
+  <si>
+    <t>CAP: Context-Aware Programming for Cyber Physical Systems</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shashank Gaur</t>
+  </si>
+  <si>
+    <t>Context-awareness is a prominently desired feature in computing systems. Smartphones, smart cards or tags, wearables, sensor nodes, and many other devices enable a system to compute context for different users and environment. With ever increasing advances in hardware for such devices, the interactions with users are increasing every day. This enables the collection of a large amount of data about users, systems, and physical environment. With such data available to be leveraged, context-awareness will soon become a necessity. Such type of data collection happens most frequently in sensing applications enabled by wireless sensor network (WSN) devices. This paper discusses the concept of context for sensing applications, specifically related to Cyber Physical Systems (CPS). The paper highlights key aspects of context and its definition. This paper proposes, to the best of the author's knowledge, the first programming approach to build context-aware applications for WSN-based CPS. This paper provides a proof of concept for a framework to detect, manage and deploy context-aware applications.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/8869350</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cyber–physical systems: Extending pervasive sensing from control theory to the Internet of Things</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BorjaBordel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Essentially, the emerging term “Cyber–Physical Systems (CPS)” is an architectural paradigm in which the pervasive sensing technologies represent a fundamental part. Originally defined in the computer sciences domain, the term Cyber–Physical Systems has been adapted to very different domains such as the control theory or electronic engineering. Even, some authors understand CPS as a particular scenario of the Internet of Things (IoT) based on pervasive sensing. Furthermore, recently, some works propose a definition for CPS including all the features described in the different domains. In this paper we provide a comprehensive analysis of the nature and characteristics of the different proposals, discuss the recent attempts to standardize CPS, and review the state-of-the-art on CPS for each technological domain. We compare those different proposals on CPS, discuss about some related terms and technologies and conclude by describing the main research challenges in the area.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1574119217303127</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Internet of Things (IoT) is a multidisciplinary tool used by field experts to fabricate technology into their discipline; these fields experts thus need access to a simple, understandable and user-friendly programming language for this purpose. Domain-Specific Languages (DSL) have been developed to pave the way for such domain experts to integrate IoT capabilities into their everyday tasks. IoT is thus one of the main technologies targeting human day-to-day activities, and the concept of IoT has caused a general rethink and reimagining of the shape of life in the future. Many researchers are thus working on fields related to IoT such as networking, power consumption, data aggregation and fusion, finding ways to offer this new technology for end user access in a smooth and easy manner. Introducing new application development methods and using software engineering standards and tools that enable end-users to develop their own IoT applications is another aspect that has received attention in the last decade; however, this aspect requires more work from the research community. The main contribution of this paper is to highlight current efforts related to the IoT field and to perform quantitative analysis to highlight the current state of the art in both positive and negative terms, including the current limitations and obstacles faced by both end-users and field experts seeking to build their own IoT applications.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://iopscience.iop.org/article/10.1088/1757-899X/1067/1/012133</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aymen J Salman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Domain-Specific Languages for IoT: Challenges and Opportunities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DSL-maps: From requirements to design of domain-specific languages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ana Pescador</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Domain-Specific Languages (DSLs) are central to Model-Driven Engineering, where they are used for creating models for particular domains. However, current research and tools for building DSLs focus on the design and implementation aspects of the DSL, while the requirements analysis phase, and its automated transition to design is largely neglected. In order to alleviate this situation, we propose DSL-maps, a notation inspired by mind-maps, to represent requirements for DSLs. The notation is supported by a tool, which helps in the automated transition into an initial meta-model design, using a customizable transformation and recommendations from a catalogue of meta-model design patterns.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/7582779</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>From sensor to situational awareness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thomas Ruth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This paper describes the integrated FlexMoT data management and visualization software system for marine sensor data. Unlike most existing solutions this software platform is designed to be neither data-centric nor visualization-centric, but seamlessly integrating both, management and visualization of measurement data. Within the project FlexMoT (Flexible Monitoring Tool) a modular, easy-to-use and fast deployable environmental monitoring solution with a high temporal and depth resolution for underwater environments has been developed. This monitoring system was designed for the use in the underwater surrounding of offshore installations like oil rigs or gas production platforms and other critical and sensitive marine environments. It enables the exact measurement of concentration of dissolved gases such as methane in water and other environmental parameters that may be indicators of leakages. The FlexMoT software stack offers situational awareness and advanced decision support in environmental monitoring by organizing, preparing and presenting the gathered sensor data in a way that (1) operator personnel of offshore installations and marine researchers can draw the right conclusions and (2) appropriate actions can be initiated swiftly and well-informed. Similar to the modular hardware approach, the software uses a plugin approach to foster the simple reconfiguration to different use-cases. The designed visualization system utilizes human perception to transform lots of data quickly and intuitively into helpful information, to draw attention to critical events or striking data and support explorative data analysis with interactive displays. The implemented visualization solution combines recent web-technologies and linked interactive 2D and 3D data presentations utilizing a direct-touch interaction metaphor. In this paper, we present the complete software stack of FlexMoT for data management, operational near real-time monitoring, visual data analytics of marine environmental data and visual forecast of gas leakage situations. It is proposed as a universal approach to improve visualization-based work with heterogeneous sensor data in environmental monitoring and marine research.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/7761249</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lantern: A domain specific language for energy awareness in smart-homes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robinson, Jon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This paper argues that energy consideration should be central to software development. It speculates that including the notion of energy awareness in programming language design for domain specific languages (DSLs) is a novel way in which energy-aware and energy-efficient applications can be developed. It outlines the design criteria and rationale for using a language-focused approach for energy-awareness. It proposes Lantern, a DSL for supporting energy awareness in Cyber-Physical Systems software development. Lantern allows the development of applications that better manage and reduce the carbon footprint of devices. The design of Lantern is aimed at supporting the general development of Cyber-Physical Systems. This paper focuses on the scenario of smart homes, using statically defined locations within a specified environment.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://content.iospress.com/articles/journal-of-ambient-intelligence-and-smart-environments/ais200580</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum-energy reprogramming with guaranteed quality-of-sensing in software-defined sensor networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deze Zeng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>After a decade of extensive research on application-specific wireless sensor networks (WSNs), the recent development of information and communication technologies make it practical to realize software-defined sensor networks (SDSNs), which are able to adapt to various application requirements and to fully explore the resources of WSNs. In SDSNs, wireless sensor nodes can be dynamically reprogrammed for different sensing tasks via the over-the-air-programming technique. For a given sensing task, it is usually required to guarantee certain quality-of-sensing, e.g., coverage ratio. Intuitively, the more sensors are deployed with a program, the higher quality-of-sensing of the corresponding task can be achieved. However, this is at the expense of high reprogramming energy consumption. In this paper, we investigate how to design an energy-efficient reprogramming strategy with guaranteed quality-of-sensing for a sensing task. To this end, two issues will be tackled: 1) the subset of sensors that shall be reprogrammed, i.e., reprogramming sensor selection and 2) the program distribution routing. They are jointly considered and formulated as an integer linear programming (ILP) problem, based on which an algorithm with low computation complexity is then proposed. The high efficiency of our algorithm is validated by extensive simulation studies.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/6883333</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self-Aware Context in Smart Home Pervasive Platforms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Philippe Lalanda</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pervasive computing envisions environments where computers are blended into everyday objects in order to provide added-value services to people. A growing number of advanced embedded systems, extended with computing and communication capabilities, are already appearing around us. However, pervasive applications raise major challenges in terms of software engineering and remain hard to develop, deploy, execute, and maintain. We believe that autonomic techniques are here needed, in particular to deal with context-awareness. In this paper, we propose to handle context management in a service-oriented pervasive platform by defining a self-aware solution and associated mechanisms. Our approach is illustrated with a smart home example implemented in our pervasive platform iCasa.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/8005340</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The common approach enabling a resource constrained device to get connected to the Internet is through programming instructions and transferring it to an embedded device. This procedure involves various tools and cross-compiling of the code depending on the platform architecture. In practical IoT applications, where a huge number of nodes exist, this process becomes almost impossible due to the heterogeneous platforms and protocols involved and the deployment conditions. This paper introduces a flexible and scalable approach that enhances modifiability and programmability through client-server-server-client architecture. It allows changing the behavior of the system after deployment through a lightweight script written with a domain specific language, DoS-IL, and stored in a gateway at the fog layer. An embedded resource browser is used to request and execute the script. The results of analysis for this model and the tools developed along the way are discussed.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behailu Negash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DoS-IL: A Domain Specific Internet of Things Language for Resource Constrained Devices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1877050917310876</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -69,7 +223,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -125,7 +279,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -412,68 +565,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="111" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="1"/>
-    <col min="2" max="2" width="67.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="176.3984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.53125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="67.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="176.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="93" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="93" customHeight="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="93" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="93" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="93" customHeight="1">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="93" customHeight="1">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="93" customHeight="1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="93" customHeight="1">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="93" customHeight="1">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C4" s="3"/>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="93" customHeight="1">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="93" customHeight="1">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>